<commit_message>
reporte por sedes listo
</commit_message>
<xml_diff>
--- a/data/2022_eje_bienestar.xlsx
+++ b/data/2022_eje_bienestar.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\svale\Desktop\RBDUOC2025\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4129880-0119-41B5-B845-30830FD6F42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E3AFAD-9FA0-4ABC-9E32-18783C44DAD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{35A884C3-4669-41DF-9DC3-61B964CD8C83}"/>
   </bookViews>
@@ -65,66 +65,6 @@
     <t>L</t>
   </si>
   <si>
-    <t>ALAMEDA</t>
-  </si>
-  <si>
-    <t>ANTONIO VARAS</t>
-  </si>
-  <si>
-    <t>CAMPUS ARAUCO</t>
-  </si>
-  <si>
-    <t>CAMPUS VILLARRICA</t>
-  </si>
-  <si>
-    <t>CONCEPCIÓN</t>
-  </si>
-  <si>
-    <t>MAIPÚ</t>
-  </si>
-  <si>
-    <t>MELIPILLA</t>
-  </si>
-  <si>
-    <t>NACIMIENTO</t>
-  </si>
-  <si>
-    <t>ONLINE</t>
-  </si>
-  <si>
-    <t>PADRE ALONSO DE OVALLE</t>
-  </si>
-  <si>
-    <t>PLAZA NORTE</t>
-  </si>
-  <si>
-    <t>PLAZA OESTE</t>
-  </si>
-  <si>
-    <t>PLAZA VESPUCIO</t>
-  </si>
-  <si>
-    <t>PUENTE ALTO</t>
-  </si>
-  <si>
-    <t>PUERTO MONTT</t>
-  </si>
-  <si>
-    <t>SAN BERNARDO</t>
-  </si>
-  <si>
-    <t>SAN CARLOS DE APOQUINDO</t>
-  </si>
-  <si>
-    <t>SAN JOAQUÍN</t>
-  </si>
-  <si>
-    <t>VALPARAÍSO</t>
-  </si>
-  <si>
-    <t>VIÑA DEL MAR</t>
-  </si>
-  <si>
     <t>Administración y Negocios</t>
   </si>
   <si>
@@ -153,6 +93,66 @@
   </si>
   <si>
     <t>Global</t>
+  </si>
+  <si>
+    <t>Alameda</t>
+  </si>
+  <si>
+    <t>Antonio Varas</t>
+  </si>
+  <si>
+    <t>Campus Arauco</t>
+  </si>
+  <si>
+    <t>Campus Villarrica</t>
+  </si>
+  <si>
+    <t>Concepción</t>
+  </si>
+  <si>
+    <t>Maipú</t>
+  </si>
+  <si>
+    <t>Melipilla</t>
+  </si>
+  <si>
+    <t>Nacimiento</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
+    <t>Padre Alonso De Ovalle</t>
+  </si>
+  <si>
+    <t>Plaza Norte</t>
+  </si>
+  <si>
+    <t>Plaza Oeste</t>
+  </si>
+  <si>
+    <t>Plaza Vespucio</t>
+  </si>
+  <si>
+    <t>Puente Alto</t>
+  </si>
+  <si>
+    <t>Puerto Montt</t>
+  </si>
+  <si>
+    <t>San Bernardo</t>
+  </si>
+  <si>
+    <t>San Carlos De Apoquindo</t>
+  </si>
+  <si>
+    <t>San Joaquín</t>
+  </si>
+  <si>
+    <t>Valparaíso</t>
+  </si>
+  <si>
+    <t>Viña Del Mar</t>
   </si>
 </sst>
 </file>
@@ -546,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C977B8F-C199-4ABB-A7AB-E3252FCC68B3}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="131" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,7 +583,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B2" s="2">
         <v>4.1302972087241496</v>
@@ -615,7 +615,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B3" s="4">
         <v>4.1516638225255971</v>
@@ -647,7 +647,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B4" s="4">
         <v>4.0955615942028984</v>
@@ -679,7 +679,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B5" s="4">
         <v>4.5769230769230766</v>
@@ -711,7 +711,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B6" s="4">
         <v>4.026209677419355</v>
@@ -743,7 +743,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B7" s="4">
         <v>3.9298469387755102</v>
@@ -775,7 +775,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B8" s="4">
         <v>4.2238756613756614</v>
@@ -807,7 +807,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B9" s="4">
         <v>4.2787698412698409</v>
@@ -839,7 +839,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B10" s="4" t="e">
         <v>#DIV/0!</v>
@@ -871,7 +871,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B11" s="4">
         <v>4.05</v>
@@ -903,7 +903,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B12" s="4">
         <v>4.1324774266365685</v>
@@ -935,7 +935,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B13" s="4">
         <v>3.8378328402366866</v>
@@ -967,7 +967,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B14" s="4">
         <v>3.9939637826961771</v>
@@ -999,7 +999,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B15" s="4">
         <v>4.0759202453987733</v>
@@ -1031,7 +1031,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B16" s="4">
         <v>4.0273876404494384</v>
@@ -1063,7 +1063,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B17" s="4">
         <v>3.9715909090909092</v>
@@ -1095,7 +1095,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B18" s="4">
         <v>4.0621584699453548</v>
@@ -1127,7 +1127,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B19" s="4">
         <v>4.0076827242524917</v>
@@ -1159,7 +1159,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B20" s="4">
         <v>4.1994540662650603</v>
@@ -1191,7 +1191,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B21" s="4">
         <v>4.2224965940054497</v>
@@ -1223,7 +1223,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B22" s="4">
         <v>4.0994759316770191</v>
@@ -1255,7 +1255,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B23" s="4">
         <v>4.2188445537065054</v>
@@ -1287,7 +1287,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B24" s="4">
         <v>3.8950825825825826</v>
@@ -1319,7 +1319,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="B25" s="4">
         <v>4.3086206896551724</v>
@@ -1351,7 +1351,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B26" s="4">
         <v>3.8597701149425285</v>
@@ -1383,7 +1383,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="B27" s="4">
         <v>4.0951640271493215</v>
@@ -1415,7 +1415,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="B28" s="4">
         <v>3.9864348142753094</v>
@@ -1447,7 +1447,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="B29" s="4">
         <v>4.2615899725274726</v>
@@ -1479,7 +1479,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B30" s="4">
         <v>4.0899898887765422</v>
@@ -1511,7 +1511,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="B31" s="4">
         <v>3.896570796460177</v>

</xml_diff>